<commit_message>
create a new folder Class and Objects
</commit_message>
<xml_diff>
--- a/13-AutomationWithPython/Exercise3/inventory.xlsx
+++ b/13-AutomationWithPython/Exercise3/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Desktop\YrkesHögskola\Software Developer Electrical &amp; Autonomus Vehicles\3- Continuous Integration\PythonTutorial\1\PythonTraining\13-AutomationWithPython\Exercise3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEDCC21-D4D5-49A1-9F1C-70EB6727FCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D195E7-FCAE-4DEE-B0D0-650E777090E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,8 +326,8 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -349,7 +349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -364,7 +364,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -378,7 +378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -420,7 +420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -434,7 +434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -448,7 +448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -462,7 +462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -504,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -532,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -546,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -574,7 +574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -602,7 +602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -616,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -630,7 +630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -644,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -658,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -672,7 +672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -686,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -700,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -714,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -742,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -756,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -770,7 +770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -784,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -798,7 +798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -812,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -826,7 +826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -840,7 +840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -854,7 +854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -868,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -890,13 +890,13 @@
         <v>458</v>
       </c>
       <c r="C40" s="2">
-        <v>200.4</v>
+        <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -924,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -938,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -952,7 +952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -966,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -980,7 +980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -994,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>688</v>
       </c>
       <c r="C63" s="2">
-        <v>55.99</v>
+        <v>5</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>4</v>
@@ -1240,7 +1240,7 @@
         <v>54</v>
       </c>
       <c r="C65" s="2">
-        <v>122.55</v>
+        <v>66</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>6</v>

</xml_diff>